<commit_message>
Removed abort(), inserted acception/rejection
</commit_message>
<xml_diff>
--- a/content/CRF_Shell/Commands_interpreter.xlsx
+++ b/content/CRF_Shell/Commands_interpreter.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Description</t>
   </si>
@@ -27,21 +27,12 @@
     <t>add an edge to the net</t>
   </si>
   <si>
-    <t>possible syntaxes</t>
-  </si>
-  <si>
     <t>add an edge to the net, assuming a simple correlation</t>
   </si>
   <si>
     <t>add an edge to the net, assuming a simple anti correlation</t>
   </si>
   <si>
-    <t>add a unary potential to the net</t>
-  </si>
-  <si>
-    <t>returns the marginals of a specified variable</t>
-  </si>
-  <si>
     <t>add the specified variables to the observed set, considering the value n as observation</t>
   </si>
   <si>
@@ -51,21 +42,6 @@
     <t>returns MAP of the actual hidden set</t>
   </si>
   <si>
-    <t>I -v:"var_name"</t>
-  </si>
-  <si>
-    <t>B -v:"name_var_a" -v:"name_var_b" -s:"../…/location of the shape .txt"</t>
-  </si>
-  <si>
-    <t>B -v:"name_var_a" -v:"name_var_b" -c:"T"</t>
-  </si>
-  <si>
-    <t>B -v:"name_var_a" -v:"name_var_b" -c:"F"</t>
-  </si>
-  <si>
-    <t>U -v:"name_var" -s:"../…/location of the shape .txt"</t>
-  </si>
-  <si>
     <t>returns the actual observed set</t>
   </si>
   <si>
@@ -75,21 +51,6 @@
     <t>clear the actual observations set, making all variables as hidden</t>
   </si>
   <si>
-    <t xml:space="preserve">S -k:"O" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">S -k:"H" </t>
-  </si>
-  <si>
-    <t>B -v:"name_var_a" -v:"name_var_b" -s:"../…/location of the shape .txt" -w:"weight_val"</t>
-  </si>
-  <si>
-    <t>B -v:"name_var_a" -v:"name_var_b" -c:"T" -w:"weight_val"</t>
-  </si>
-  <si>
-    <t>B -v:"name_var_a" -v:"name_var_b" -c:"F" -w:"weight_val"</t>
-  </si>
-  <si>
     <t>add an edge to the net, considering an exponential potential with w as weight</t>
   </si>
   <si>
@@ -99,43 +60,73 @@
     <t>add an edge to the net, assuming a simple anti correlation, considering an exponential potential with w as weight</t>
   </si>
   <si>
-    <t>X -p:"config.xml" -f:"C:/…../fldkjkdf/jfdhjdf/"</t>
-  </si>
-  <si>
     <t>clean attual graph and rebuild reading that config file. P is the name of the xml, while f is the folder where is contained</t>
   </si>
   <si>
-    <t>U -v:"name_var" -s:"../…/location of the shape .txt" -w:"weight_val"</t>
-  </si>
-  <si>
-    <t>add a unary potential to the net, considering an exponential potential</t>
-  </si>
-  <si>
-    <t>O -v:"observ_1" -n:"2"  -v:"observ_2" -n:"0" -v:"observ_3" -n:"1"</t>
-  </si>
-  <si>
     <t>O</t>
   </si>
   <si>
     <t>Create the specified new variables, in order to insert new potentials in the future referring to them</t>
   </si>
   <si>
-    <t>C -f:"../../jkjkj/commands_sequence"</t>
-  </si>
-  <si>
     <t>execute the sequence of commands contained in the specified textual file</t>
   </si>
   <si>
-    <t>V  -v:"name_var_a" -s:"size_var_a"-v:"name_var_b" -s:"size_var_b" …</t>
-  </si>
-  <si>
     <t xml:space="preserve">launch the interface </t>
   </si>
   <si>
     <t xml:space="preserve">J </t>
   </si>
   <si>
-    <t xml:space="preserve">V </t>
+    <t>get the JSON describing the actual graph</t>
+  </si>
+  <si>
+    <t>X $ p $ config.xml $ f $ C:/…../fldkjkdf/jfdhjdf/</t>
+  </si>
+  <si>
+    <t>V $ v $ name_a $ s $ size_a $ v $ name_b $ s $ size_b</t>
+  </si>
+  <si>
+    <t>P $ v $ name_var_a $ v $ name_var_b $ s $ ../…/location of the shape .txt $ w $ weight_val</t>
+  </si>
+  <si>
+    <t>P $ v $ name_var_a $ v $ name_var_b $ c $ T $ w $ weight_val</t>
+  </si>
+  <si>
+    <t>P $ v $ name_var_a $ v $ name_var_b $ c $ F$ w $ weight_val</t>
+  </si>
+  <si>
+    <t>P $ v $ name_var_a $ v $ name_var_b $ s $ ../…/location of the shape .txt</t>
+  </si>
+  <si>
+    <t>P $ v $ name_var_a $ v $ name_var_b $  c $ T</t>
+  </si>
+  <si>
+    <t>P $ v $ name_var_a $ v $ name_var_b $ c $ F</t>
+  </si>
+  <si>
+    <t>O $ v $ observ_1 $ n $ 2 $ v $ observ_2 $ n $ 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S $ k $ O </t>
+  </si>
+  <si>
+    <t xml:space="preserve">S $ k $ H </t>
+  </si>
+  <si>
+    <t>possible syntaxes: substitute ' $ ' -&gt; '$'</t>
+  </si>
+  <si>
+    <t>returns the marginals of specified variables</t>
+  </si>
+  <si>
+    <t>I  $ v $ var_name_A $ v $ var_name_B</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>B $ f $ ../../jkjkj/commands_sequence</t>
   </si>
 </sst>
 </file>
@@ -179,12 +170,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF66FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF9966"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -222,6 +207,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -263,10 +254,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -582,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,7 +591,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -610,49 +603,49 @@
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>36</v>
+      <c r="A5" s="12" t="s">
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>2</v>
@@ -660,111 +653,101 @@
     </row>
     <row r="11" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>30</v>
+        <v>15</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18"/>
+    </row>
+    <row r="19" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21"/>
     </row>
     <row r="22" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>10</v>
-      </c>
+    </row>
+    <row r="23" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+      <c r="B26" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B28" s="2"/>
-    </row>
-    <row r="29" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Possibility to save a model in an xml file (Reprint) Inserted
</commit_message>
<xml_diff>
--- a/content/CRF_Shell/Commands_interpreter.xlsx
+++ b/content/CRF_Shell/Commands_interpreter.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Description</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>Add to the actual net the components contained in the graph described by a config file</t>
+  </si>
+  <si>
+    <t>Print the actual structure into the specified configuration file</t>
+  </si>
+  <si>
+    <t>R $ f $ config.xml</t>
   </si>
 </sst>
 </file>
@@ -155,7 +161,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,6 +231,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF66FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -256,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -273,6 +285,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -281,6 +294,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF66FF"/>
       <color rgb="FF9F9409"/>
       <color rgb="FF85E307"/>
       <color rgb="FFFF9900"/>
@@ -289,7 +303,6 @@
       <color rgb="FFFF0000"/>
       <color rgb="FFFFFF66"/>
       <color rgb="FFFF9966"/>
-      <color rgb="FFFF66FF"/>
       <color rgb="FF66CCFF"/>
     </mruColors>
   </colors>
@@ -588,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,6 +782,14 @@
       </c>
       <c r="B30" s="2" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>